<commit_message>
get rid of unnecessary bom/place files. update atgm336h file to 180 rotation for U5 gps chip
</commit_message>
<xml_diff>
--- a/tracker/pcb/tracker/v0.4_kbn/PickAndPlace_PCB1_2023-09-11_atgm336h-5n31.xlsx
+++ b/tracker/pcb/tracker/v0.4_kbn/PickAndPlace_PCB1_2023-09-11_atgm336h-5n31.xlsx
@@ -773,8 +773,8 @@
   </sheetPr>
   <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -886,7 +886,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>